<commit_message>
initial commit of xml parser. fix color of unselected text in navigation drawer.
</commit_message>
<xml_diff>
--- a/doc/DBSpreadsheet.xlsx
+++ b/doc/DBSpreadsheet.xlsx
@@ -23,8 +23,19 @@
 </workbook>
 </file>
 
+<file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <connection id="1" name="DBSchema" type="4" refreshedVersion="0" background="1">
+    <webPr xml="1" sourceData="1" url="D:\Projects\aerial-genie\doc\DBSchema.xml" htmlTables="1" htmlFormat="all"/>
+  </connection>
+  <connection id="2" name="DBSchema1" type="4" refreshedVersion="0" background="1">
+    <webPr xml="1" sourceData="1" url="D:\Projects\aerial-genie\doc\DBSchema.xml" htmlTables="1" htmlFormat="all"/>
+  </connection>
+</connections>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>id</t>
   </si>
@@ -36,6 +47,36 @@
   </si>
   <si>
     <t>Ballerina</t>
+  </si>
+  <si>
+    <t>Fireman Spin</t>
+  </si>
+  <si>
+    <t>Twisted Ballerina</t>
+  </si>
+  <si>
+    <t>Basic Invert</t>
+  </si>
+  <si>
+    <t>Jasmine</t>
+  </si>
+  <si>
+    <t>Superman</t>
+  </si>
+  <si>
+    <t>Cupid</t>
+  </si>
+  <si>
+    <t>Butterfly</t>
+  </si>
+  <si>
+    <t>Wrist Seat</t>
+  </si>
+  <si>
+    <t>Genie</t>
+  </si>
+  <si>
+    <t>http://i.imgur.com/vckohBE.jpg</t>
   </si>
 </sst>
 </file>
@@ -71,8 +112,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -88,6 +130,51 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/xmlMaps.xml><?xml version="1.0" encoding="utf-8"?>
+<MapInfo xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" SelectionNamespaces="">
+  <Schema ID="Schema2">
+    <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns="">
+      <xsd:element nillable="true" name="moveset">
+        <xsd:complexType>
+          <xsd:sequence minOccurs="0">
+            <xsd:element minOccurs="0" maxOccurs="unbounded" nillable="true" name="move" form="unqualified">
+              <xsd:complexType>
+                <xsd:sequence minOccurs="0">
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:integer" name="id" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="name" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="img" form="unqualified"/>
+                </xsd:sequence>
+              </xsd:complexType>
+            </xsd:element>
+          </xsd:sequence>
+        </xsd:complexType>
+      </xsd:element>
+    </xsd:schema>
+  </Schema>
+  <Map ID="2" Name="moveset_Map" RootElement="moveset" SchemaID="Schema2" ShowImportExportValidationErrors="false" AutoFit="true" Append="false" PreserveSortAFLayout="true" PreserveFormat="true">
+    <DataBinding FileBinding="true" ConnectionID="2" DataBindingLoadMode="1"/>
+  </Map>
+</MapInfo>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:C11" tableType="xml" totalsRowShown="0" connectionId="2">
+  <autoFilter ref="A1:C11"/>
+  <tableColumns count="3">
+    <tableColumn id="1" uniqueName="id" name="id">
+      <xmlColumnPr mapId="2" xpath="/moveset/move/id" xmlDataType="integer"/>
+    </tableColumn>
+    <tableColumn id="2" uniqueName="name" name="name">
+      <xmlColumnPr mapId="2" xpath="/moveset/move/name" xmlDataType="string"/>
+    </tableColumn>
+    <tableColumn id="3" uniqueName="img" name="img">
+      <xmlColumnPr mapId="2" xpath="/moveset/move/img" xmlDataType="string"/>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -353,13 +440,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.28515625" customWidth="1"/>
+    <col min="3" max="3" width="6.5703125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -373,11 +465,102 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="C2" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="1"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="1"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="1"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="1"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="1"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="1"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="1"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="1"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added recyclerview test layout and picasso support
</commit_message>
<xml_diff>
--- a/doc/DBSpreadsheet.xlsx
+++ b/doc/DBSpreadsheet.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>id</t>
   </si>
@@ -76,13 +76,40 @@
     <t>Genie</t>
   </si>
   <si>
-    <t>http://i.imgur.com/vckohBE.jpg</t>
+    <t>http://i.imgur.com/zGvSDQJ.jpg</t>
+  </si>
+  <si>
+    <t>http://i.imgur.com/PUf63rI.jpg</t>
+  </si>
+  <si>
+    <t>http://i.imgur.com/fGrAGrb.png</t>
+  </si>
+  <si>
+    <t>http://i.imgur.com/VemIfxQ.jpg</t>
+  </si>
+  <si>
+    <t>http://i.imgur.com/EV5VY5m.jpg</t>
+  </si>
+  <si>
+    <t>http://i.imgur.com/WIHKX5U.jpg</t>
+  </si>
+  <si>
+    <t>http://i.imgur.com/pKI3a3m.jpg</t>
+  </si>
+  <si>
+    <t>http://i.imgur.com/pS1Q1Qa.jpg</t>
+  </si>
+  <si>
+    <t>http://i.imgur.com/i2Fo7PN.jpg</t>
+  </si>
+  <si>
+    <t>http://i.imgur.com/nenXqc0.jpg</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -253,6 +280,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -288,6 +332,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -443,7 +504,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -482,7 +543,9 @@
       <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="1"/>
+      <c r="C3" s="1" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
@@ -491,7 +554,9 @@
       <c r="B4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="1"/>
+      <c r="C4" s="1" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
@@ -500,7 +565,9 @@
       <c r="B5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="1"/>
+      <c r="C5" s="1" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
@@ -509,7 +576,9 @@
       <c r="B6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="1"/>
+      <c r="C6" s="1" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
@@ -518,7 +587,9 @@
       <c r="B7" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="1"/>
+      <c r="C7" s="1" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
@@ -527,7 +598,9 @@
       <c r="B8" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="1"/>
+      <c r="C8" s="1" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
@@ -536,7 +609,9 @@
       <c r="B9" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="1"/>
+      <c r="C9" s="1" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
@@ -545,7 +620,9 @@
       <c r="B10" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="1"/>
+      <c r="C10" s="1" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
@@ -554,7 +631,9 @@
       <c r="B11" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="1"/>
+      <c r="C11" s="1" t="s">
+        <v>22</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>